<commit_message>
Added fixation and feedback
</commit_message>
<xml_diff>
--- a/block_params.xlsx
+++ b/block_params.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macuser/Documents/PYTHON/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34F8C18B-6908-CB49-997C-100F1E845F12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED8A4C8-06AC-EA42-BFA4-8052845730BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1280" yWindow="1960" windowWidth="24240" windowHeight="13500" xr2:uid="{5FC487F5-469A-3049-A530-ADFE4209F517}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>condsFile</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>block2_params.xlsx</t>
+  </si>
+  <si>
+    <t>block3_params.xlsx</t>
   </si>
 </sst>
 </file>
@@ -391,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3779AE0A-4F30-794C-8F96-D68F0113E4D2}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -414,6 +417,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>